<commit_message>
TA27,28,29,30,31 IC Front End Update(Complete)
Note the sheet it refers to is jdgroupleverchTA15.
Observe the report how data displays as per pass/fail scenarios.
Review Comments in sheet to understand execution flow and how to execute
scenarios
</commit_message>
<xml_diff>
--- a/src/test/resources/data/jdgroupleverchTA15.xlsx
+++ b/src/test/resources/data/jdgroupleverchTA15.xlsx
@@ -3,27 +3,64 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21727"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9CBB127-FC1F-494E-9202-44033B88E5D8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CADC4714-DA44-4974-BFF7-813F78BEB2CC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Suites" sheetId="22" r:id="rId1"/>
     <sheet name="IC" sheetId="23" r:id="rId2"/>
     <sheet name="accountCreation++" sheetId="31" r:id="rId3"/>
-    <sheet name="Login++" sheetId="25" r:id="rId4"/>
-    <sheet name="Russels" sheetId="26" r:id="rId5"/>
-    <sheet name="Bradlows" sheetId="27" r:id="rId6"/>
-    <sheet name="Rochester" sheetId="28" r:id="rId7"/>
-    <sheet name="Sleepmasters" sheetId="29" r:id="rId8"/>
-    <sheet name="HiFiCorp" sheetId="30" r:id="rId9"/>
+    <sheet name="Login_magento++" sheetId="32" r:id="rId4"/>
+    <sheet name="Login++" sheetId="25" r:id="rId5"/>
+    <sheet name="Russels" sheetId="26" r:id="rId6"/>
+    <sheet name="Bradlows" sheetId="27" r:id="rId7"/>
+    <sheet name="Rochester" sheetId="28" r:id="rId8"/>
+    <sheet name="Sleepmasters" sheetId="29" r:id="rId9"/>
+    <sheet name="HiFiCorp" sheetId="30" r:id="rId10"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={F7FEE7C6-09DD-46F2-8FBC-7A3D99E4B086}</author>
+    <author>tc={92C9AF37-2008-4E76-9819-2636A9024A9D}</author>
+    <author>tc={049E9369-0946-4F59-9241-B6CC037A7AA7}</author>
+  </authors>
+  <commentList>
+    <comment ref="H2" authorId="0" shapeId="0" xr:uid="{F7FEE7C6-09DD-46F2-8FBC-7A3D99E4B086}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    For Vat Number ensure that column I is populated with information otherwise it will fail</t>
+      </text>
+    </comment>
+    <comment ref="H3" authorId="1" shapeId="0" xr:uid="{92C9AF37-2008-4E76-9819-2636A9024A9D}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    If flag is set to ID make sure that identityType is set to ID</t>
+      </text>
+    </comment>
+    <comment ref="H5" authorId="2" shapeId="0" xr:uid="{049E9369-0946-4F59-9241-B6CC037A7AA7}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    If flag is set to newsletter, note in column K. If set to YES it expects H to be set to Newsletter otherwise it will fail - The same vice versa applies to No Newsletter</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="92">
   <si>
     <t>Execute</t>
   </si>
@@ -157,9 +194,6 @@
     <t>testCaseName</t>
   </si>
   <si>
-    <t>Create new customer in IC</t>
-  </si>
-  <si>
     <t>firstName</t>
   </si>
   <si>
@@ -175,59 +209,140 @@
     <t>vatNumber</t>
   </si>
   <si>
+    <t>identityType</t>
+  </si>
+  <si>
+    <t>accountCreation</t>
+  </si>
+  <si>
+    <t>Jones</t>
+  </si>
+  <si>
+    <t>identityNumber/passport</t>
+  </si>
+  <si>
+    <t>validatePassword</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>validateIncorrectID</t>
+  </si>
+  <si>
+    <t>validateIDWithMoreDigits</t>
+  </si>
+  <si>
+    <t>validateIDWithLessDigits</t>
+  </si>
+  <si>
+    <t>Brian</t>
+  </si>
+  <si>
+    <t>validateExistingAccount</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>https://staging-jdgroup-m23.vaimo.net/T5sjY7drHkyB6Z4n/admin/index/index/key/4cee16108e07c6904ab12f33e9f10b9b1b1fadb7c06faa4c94fbd03a1d1018ff/</t>
+  </si>
+  <si>
+    <t>Access#11</t>
+  </si>
+  <si>
+    <t>Create new customer in IC and Validate Vat Number</t>
+  </si>
+  <si>
+    <t>Password2</t>
+  </si>
+  <si>
+    <t>5311266534086</t>
+  </si>
+  <si>
+    <t>Password3</t>
+  </si>
+  <si>
+    <t>WebSite</t>
+  </si>
+  <si>
+    <t>Incredible Connection</t>
+  </si>
+  <si>
+    <t>verficationFlag</t>
+  </si>
+  <si>
     <t>newsletter</t>
   </si>
   <si>
-    <t>identityType</t>
-  </si>
-  <si>
-    <t>accountCreation</t>
-  </si>
-  <si>
-    <t>Jones</t>
+    <t>Passport</t>
+  </si>
+  <si>
+    <t>Newsletter</t>
+  </si>
+  <si>
+    <t>Vat Number</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>No newsletter</t>
   </si>
   <si>
     <t>Yes</t>
   </si>
   <si>
-    <t>identityNumber/passport</t>
-  </si>
-  <si>
-    <t>validatePassword</t>
-  </si>
-  <si>
-    <t>James12Runs</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>validateIncorrectID</t>
-  </si>
-  <si>
-    <t>validateIDWithMoreDigits</t>
-  </si>
-  <si>
-    <t>validateIDWithLessDigits</t>
-  </si>
-  <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>Brian</t>
-  </si>
-  <si>
-    <t>validateExistingAccount</t>
-  </si>
-  <si>
-    <t>BrenoFernandesRochddas@armyspy.com</t>
+    <t>Create new customer in IC and Validate ID</t>
+  </si>
+  <si>
+    <t>Create new customer in IC and Validate passport</t>
+  </si>
+  <si>
+    <t>Create new customer in IC and Validate Newsletter Without subscription</t>
+  </si>
+  <si>
+    <t>Create new customer in IC and Validate newsletter with no subscription</t>
+  </si>
+  <si>
+    <t>Create new customer in IC and Validate with no subscription and do not subscribe</t>
+  </si>
+  <si>
+    <t>Create new customer in IC and Validate Newsletter as well as subscribe</t>
+  </si>
+  <si>
+    <t>BrenoFernandesMalingaPatrick29@armyspy.com</t>
+  </si>
+  <si>
+    <t>BrenoFernandesMalingaPatrick30@armyspy.com</t>
+  </si>
+  <si>
+    <t>BrenoFernandesMalingaPatrick31@armyspy.com</t>
+  </si>
+  <si>
+    <t>BrenoFernandesMalingaPatrick32@armyspy.com</t>
+  </si>
+  <si>
+    <t>BrenoFernandesMalingaPatrick33@armyspy.com</t>
+  </si>
+  <si>
+    <t>BrenoFernandesMalingaPatrick34@armyspy.com</t>
+  </si>
+  <si>
+    <t>BrenoFernandesMalingaPatrick35@armyspy.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -249,6 +364,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -272,18 +393,90 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="7">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -294,6 +487,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -615,6 +812,20 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="H2" dT="2021-02-18T18:48:21.98" personId="{00000000-0000-0000-0000-000000000000}" id="{F7FEE7C6-09DD-46F2-8FBC-7A3D99E4B086}">
+    <text>For Vat Number ensure that column I is populated with information otherwise it will fail</text>
+  </threadedComment>
+  <threadedComment ref="H3" dT="2021-02-18T18:45:35.46" personId="{00000000-0000-0000-0000-000000000000}" id="{92C9AF37-2008-4E76-9819-2636A9024A9D}">
+    <text>If flag is set to ID make sure that identityType is set to ID</text>
+  </threadedComment>
+  <threadedComment ref="H5" dT="2021-02-18T18:47:39.22" personId="{00000000-0000-0000-0000-000000000000}" id="{049E9369-0946-4F59-9241-B6CC037A7AA7}">
+    <text>If flag is set to newsletter, note in column K. If set to YES it expects H to be set to Newsletter otherwise it will fail - The same vice versa applies to No Newsletter</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G7"/>
@@ -779,21 +990,125 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:M5"/>
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="12" width="7.7265625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.7265625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:M10"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="62" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19" style="1" customWidth="1"/>
     <col min="4" max="5" width="26.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.6328125" bestFit="1" customWidth="1"/>
     <col min="7" max="12" width="7.7265625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="8.7265625" bestFit="1" customWidth="1"/>
   </cols>
@@ -881,31 +1196,133 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>44</v>
+        <v>65</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D4" t="s">
-        <v>52</v>
+      <c r="D4" s="1" t="s">
+        <v>50</v>
       </c>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="D5" s="1"/>
+    <row r="5" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>50</v>
+      </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="E4:F4">
+    <cfRule type="duplicateValues" dxfId="6" priority="7"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E5:F5">
+    <cfRule type="duplicateValues" dxfId="5" priority="6"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E6:F6">
+    <cfRule type="duplicateValues" dxfId="4" priority="5"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E7:F7">
+    <cfRule type="duplicateValues" dxfId="3" priority="4"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E8:F8">
+    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E9:F9">
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E10:F10">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5054DFA-212C-4ABC-86D1-7A882998953C}">
-  <dimension ref="A1:P2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5054DFA-212C-4ABC-86D1-7A882998953C}">
+  <dimension ref="A1:R8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -917,17 +1334,19 @@
     <col min="5" max="5" width="33.08984375" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.1796875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="22.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.6328125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.08984375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.26953125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22.26953125" style="1" customWidth="1"/>
-    <col min="13" max="13" width="15.453125" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="23.26953125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="17.26953125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.453125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.1796875" style="1" customWidth="1"/>
+    <col min="12" max="12" width="11.08984375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22.26953125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="22.26953125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="23.26953125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>38</v>
       </c>
@@ -935,49 +1354,55 @@
         <v>36</v>
       </c>
       <c r="C1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" t="s">
         <v>45</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>47</v>
       </c>
       <c r="F1" t="s">
         <v>21</v>
       </c>
       <c r="G1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="I1" t="s">
         <v>48</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="L1" t="s">
         <v>49</v>
       </c>
-      <c r="I1" t="s">
-        <v>50</v>
-      </c>
-      <c r="J1" t="s">
-        <v>51</v>
-      </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
+        <v>52</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="O1" t="s">
+        <v>53</v>
+      </c>
+      <c r="P1" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>56</v>
+      </c>
+      <c r="R1" t="s">
         <v>55</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="M1" t="s">
-        <v>56</v>
-      </c>
-      <c r="N1" t="s">
-        <v>61</v>
-      </c>
-      <c r="O1" t="s">
-        <v>60</v>
-      </c>
-      <c r="P1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>3</v>
       </c>
@@ -985,66 +1410,512 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>65</v>
+        <v>85</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="G2" t="s">
-        <v>57</v>
-      </c>
-      <c r="I2" t="s">
-        <v>54</v>
-      </c>
-      <c r="J2" t="s">
-        <v>62</v>
-      </c>
-      <c r="K2">
-        <v>5311266534086</v>
-      </c>
-      <c r="L2" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="I2">
+        <v>2222224</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="L2" t="s">
+        <v>76</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="O2" t="s">
+        <v>54</v>
+      </c>
+      <c r="P2" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>54</v>
+      </c>
+      <c r="R2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="1">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="M2" t="s">
+      <c r="D3" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I3" s="1">
+        <v>2222224</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="M3" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="1">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="N2" t="s">
+      <c r="D4" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="I4" s="1">
+        <v>2222224</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="M4" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="1">
+        <v>6</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="O2" t="s">
+      <c r="D5" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I5" s="1">
+        <v>2222224</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="M5" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="1">
+        <v>7</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="P2" t="s">
+      <c r="D6" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="I6" s="1">
+        <v>2222224</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="M6" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="R6" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="1">
+        <v>8</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>58</v>
       </c>
+      <c r="D7" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="I7" s="1">
+        <v>2222224</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="M7" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="R7" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="1">
+        <v>9</v>
+      </c>
+      <c r="B8" s="1">
+        <v>1</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I8" s="1">
+        <v>2222224</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="M8" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="R8" s="1" t="s">
+        <v>54</v>
+      </c>
     </row>
   </sheetData>
-  <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2" xr:uid="{7E4ACF57-A660-45A6-807C-8A457DFE8ACC}">
-      <formula1>"Yes,No"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2" xr:uid="{3298DDCC-15EA-4EE3-A635-A5C0AB2F4931}">
+  <dataValidations count="4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L8" xr:uid="{3298DDCC-15EA-4EE3-A635-A5C0AB2F4931}">
       <formula1>"ID, Passport"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2 N2 O2 P2 L2" xr:uid="{C9501321-A586-4737-BFCB-117928C244E7}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2:R8 K2:K8" xr:uid="{C9501321-A586-4737-BFCB-117928C244E7}">
       <formula1>"Yes, No"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J8" xr:uid="{A768279C-3465-4C38-BACE-AE576B0A5FF2}">
+      <formula1>"Main Website,Incredible Connection,Hifi Corporation,Russells,Sleepmasters,Rochester"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H8" xr:uid="{D42F678B-31D0-47DE-8C88-07AD2C43E093}">
+      <formula1>"Vat Number,ID,Passport,Newsletter,No newsletter"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" xr:uid="{AB8E7C76-B0AF-4A29-BC65-B8C633EFAC74}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{AD535C4E-CAA2-4CB7-9267-DBFDB9FD9D6C}"/>
+    <hyperlink ref="E4" r:id="rId3" xr:uid="{C3A9B660-FA3F-470D-8386-197E36F4FE59}"/>
+    <hyperlink ref="E5" r:id="rId4" xr:uid="{44658958-BA2D-427F-9C49-0028D635EE29}"/>
+    <hyperlink ref="E6" r:id="rId5" xr:uid="{830BF3D2-A4C7-42D2-A971-0E94942E692C}"/>
+    <hyperlink ref="E7" r:id="rId6" xr:uid="{2C797534-05B6-4B1F-9BA9-3976F805D67C}"/>
+    <hyperlink ref="E8" r:id="rId7" xr:uid="{1F87E4B2-E0DF-411D-8AD5-825D94C91A22}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId8"/>
+  <legacyDrawing r:id="rId9"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABC47B48-85A6-4DB0-B46C-2C974E03CC91}">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="9.1796875" style="1"/>
+    <col min="2" max="2" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="144.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.1796875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D2" s="1">
+        <v>225564</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D3" s="1">
+        <v>225564</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D4" s="1">
+        <v>225504</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D13"/>
   <sheetViews>
@@ -1248,7 +2119,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:N3"/>
   <sheetViews>
@@ -1353,7 +2224,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:M3"/>
   <sheetViews>
@@ -1457,7 +2328,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:M3"/>
   <sheetViews>
@@ -1561,7 +2432,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:M3"/>
   <sheetViews>
@@ -1663,108 +2534,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:M3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="12" width="7.7265625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.7265625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
TA27,28,29,30,31 IC Front end update(Completed)
Refers to sheet jdgroupleverchTA15.xlsx
</commit_message>
<xml_diff>
--- a/src/test/resources/data/jdgroupleverchTA15.xlsx
+++ b/src/test/resources/data/jdgroupleverchTA15.xlsx
@@ -3,27 +3,28 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21727"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9CBB127-FC1F-494E-9202-44033B88E5D8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6126B909-277E-464C-96E6-F465C7E80639}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Suites" sheetId="22" r:id="rId1"/>
     <sheet name="IC" sheetId="23" r:id="rId2"/>
-    <sheet name="accountCreation++" sheetId="31" r:id="rId3"/>
-    <sheet name="Login++" sheetId="25" r:id="rId4"/>
-    <sheet name="Russels" sheetId="26" r:id="rId5"/>
-    <sheet name="Bradlows" sheetId="27" r:id="rId6"/>
-    <sheet name="Rochester" sheetId="28" r:id="rId7"/>
-    <sheet name="Sleepmasters" sheetId="29" r:id="rId8"/>
-    <sheet name="HiFiCorp" sheetId="30" r:id="rId9"/>
+    <sheet name="accountCreation++" sheetId="33" r:id="rId3"/>
+    <sheet name="Login_magento++" sheetId="32" r:id="rId4"/>
+    <sheet name="Login++" sheetId="25" r:id="rId5"/>
+    <sheet name="Russels" sheetId="26" r:id="rId6"/>
+    <sheet name="Bradlows" sheetId="27" r:id="rId7"/>
+    <sheet name="Rochester" sheetId="28" r:id="rId8"/>
+    <sheet name="Sleepmasters" sheetId="29" r:id="rId9"/>
+    <sheet name="HiFiCorp" sheetId="30" r:id="rId10"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="90">
   <si>
     <t>Execute</t>
   </si>
@@ -157,9 +158,6 @@
     <t>testCaseName</t>
   </si>
   <si>
-    <t>Create new customer in IC</t>
-  </si>
-  <si>
     <t>firstName</t>
   </si>
   <si>
@@ -187,40 +185,115 @@
     <t>Jones</t>
   </si>
   <si>
+    <t>identityNumber/passport</t>
+  </si>
+  <si>
+    <t>validatePassword</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>validateIncorrectID</t>
+  </si>
+  <si>
+    <t>validateIDWithMoreDigits</t>
+  </si>
+  <si>
+    <t>validateIDWithLessDigits</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Brian</t>
+  </si>
+  <si>
+    <t>validateExistingAccount</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>https://staging-jdgroup-m23.vaimo.net/T5sjY7drHkyB6Z4n/admin/index/index/key/4cee16108e07c6904ab12f33e9f10b9b1b1fadb7c06faa4c94fbd03a1d1018ff/</t>
+  </si>
+  <si>
+    <t>Access#11</t>
+  </si>
+  <si>
+    <t>Create new customer in IC and Validate Vat Number</t>
+  </si>
+  <si>
+    <t>Password2</t>
+  </si>
+  <si>
+    <t>5311266534086</t>
+  </si>
+  <si>
+    <t>Password3</t>
+  </si>
+  <si>
+    <t>WebSite</t>
+  </si>
+  <si>
+    <t>Incredible Connection</t>
+  </si>
+  <si>
+    <t>vatNumberFlag</t>
+  </si>
+  <si>
     <t>Yes</t>
   </si>
   <si>
-    <t>identityNumber/passport</t>
-  </si>
-  <si>
-    <t>validatePassword</t>
-  </si>
-  <si>
-    <t>James12Runs</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>validateIncorrectID</t>
-  </si>
-  <si>
-    <t>validateIDWithMoreDigits</t>
-  </si>
-  <si>
-    <t>validateIDWithLessDigits</t>
-  </si>
-  <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>Brian</t>
-  </si>
-  <si>
-    <t>validateExistingAccount</t>
-  </si>
-  <si>
-    <t>BrenoFernandesRochddas@armyspy.com</t>
+    <t>Create new customer in IC and Validate VAT Number</t>
+  </si>
+  <si>
+    <t>TestCaseName</t>
+  </si>
+  <si>
+    <t>Create new customer in IC and Validate ID number</t>
+  </si>
+  <si>
+    <t>Create new customer in IC and Validate Passport</t>
+  </si>
+  <si>
+    <t>Create new customer in IC and Validate With NewsLetter</t>
+  </si>
+  <si>
+    <t>Create new customer in IC and Validate Without newsletter</t>
+  </si>
+  <si>
+    <t>Create new customer in IC and Validate ID Number</t>
+  </si>
+  <si>
+    <t>Create new customer in IC and Validate with newsletter</t>
+  </si>
+  <si>
+    <t>Create new customer in IC and Validate without newsletter</t>
+  </si>
+  <si>
+    <t>BrenoFernandesMalingaPatrick82@armyspy.com</t>
+  </si>
+  <si>
+    <t>BrenoFernandesMalingaPatrick83@armyspy.com</t>
+  </si>
+  <si>
+    <t>BrenoFernandesMalingaPatrick85@armyspy.com</t>
+  </si>
+  <si>
+    <t>BrenoFernandesMalingaPatrick86@armyspy.com</t>
+  </si>
+  <si>
+    <t>Passport</t>
+  </si>
+  <si>
+    <t>BrenoFernandesMalingaPatrick87@armyspy.com</t>
   </si>
 </sst>
 </file>
@@ -277,13 +350,64 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="5">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -779,21 +903,125 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:M5"/>
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="12" width="7.7265625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.7265625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:M8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.6328125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19" style="1" customWidth="1"/>
     <col min="4" max="5" width="26.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.6328125" bestFit="1" customWidth="1"/>
     <col min="7" max="12" width="7.7265625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="8.7265625" bestFit="1" customWidth="1"/>
   </cols>
@@ -881,170 +1109,597 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>44</v>
+        <v>67</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D4" t="s">
-        <v>52</v>
+      <c r="D4" s="1" t="s">
+        <v>51</v>
       </c>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="D5" s="1"/>
+    <row r="5" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>51</v>
+      </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="E4:F4 E5:E8">
+    <cfRule type="duplicateValues" dxfId="4" priority="5"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F5">
+    <cfRule type="duplicateValues" dxfId="3" priority="4"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F6">
+    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F7">
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F8">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5054DFA-212C-4ABC-86D1-7A882998953C}">
-  <dimension ref="A1:P2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCA23956-C18F-403E-98A2-D08FD3557824}">
+  <dimension ref="A1:S6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="33.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.1796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.6328125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.08984375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.26953125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22.26953125" style="1" customWidth="1"/>
-    <col min="13" max="13" width="15.453125" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="23.26953125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="17.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="48.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.453125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="10.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="22.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="22.26953125" style="1" customWidth="1"/>
+    <col min="16" max="16" width="15.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="23.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="17.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="F1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="I1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="I1" t="s">
+      <c r="M1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="J1" t="s">
-        <v>51</v>
-      </c>
-      <c r="K1" t="s">
-        <v>55</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="M1" t="s">
+      <c r="N1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="N1" t="s">
-        <v>61</v>
-      </c>
-      <c r="O1" t="s">
-        <v>60</v>
-      </c>
-      <c r="P1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>3</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
-        <v>63</v>
+      <c r="C2" s="1" t="s">
+        <v>75</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="G2" t="s">
-        <v>57</v>
-      </c>
-      <c r="I2" t="s">
-        <v>54</v>
-      </c>
-      <c r="J2" t="s">
-        <v>62</v>
-      </c>
-      <c r="K2">
-        <v>5311266534086</v>
+        <v>60</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J2" s="1">
+        <v>2222224</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>72</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="M2" t="s">
-        <v>58</v>
-      </c>
-      <c r="N2" t="s">
-        <v>58</v>
-      </c>
-      <c r="O2" t="s">
-        <v>58</v>
-      </c>
-      <c r="P2" t="s">
-        <v>58</v>
+        <v>55</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A3" s="1">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J3" s="1">
+        <v>2222224</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A4" s="1">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J4" s="1">
+        <v>2222224</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="N4" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A5" s="1">
+        <v>6</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J5" s="1">
+        <v>2222224</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="N5" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A6" s="1">
+        <v>7</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J6" s="1">
+        <v>2222224</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="N6" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="R6" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2" xr:uid="{7E4ACF57-A660-45A6-807C-8A457DFE8ACC}">
-      <formula1>"Yes,No"</formula1>
+  <dataValidations count="4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K6" xr:uid="{A768279C-3465-4C38-BACE-AE576B0A5FF2}">
+      <formula1>"Main Website,Incredible Connection,Hifi Corporation,Russells,Sleepmasters,Rochester"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2" xr:uid="{3298DDCC-15EA-4EE3-A635-A5C0AB2F4931}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O2:S6 I2:I6" xr:uid="{C9501321-A586-4737-BFCB-117928C244E7}">
+      <formula1>"Yes, No"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2:M6" xr:uid="{3298DDCC-15EA-4EE3-A635-A5C0AB2F4931}">
       <formula1>"ID, Passport"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2 N2 O2 P2 L2" xr:uid="{C9501321-A586-4737-BFCB-117928C244E7}">
-      <formula1>"Yes, No"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L6" xr:uid="{7E4ACF57-A660-45A6-807C-8A457DFE8ACC}">
+      <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{AB8E7C76-B0AF-4A29-BC65-B8C633EFAC74}"/>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{F4AF6A03-1E86-46D8-ADF4-019927046C92}"/>
+    <hyperlink ref="F3" r:id="rId2" xr:uid="{DEB66DB2-3314-416A-9607-BB82BB76055B}"/>
+    <hyperlink ref="F5" r:id="rId3" xr:uid="{71909ED7-5D76-475B-9E35-5ED0D5647811}"/>
+    <hyperlink ref="F6" r:id="rId4" xr:uid="{335EFCA3-2C02-4FDA-9713-29BF0B7A239B}"/>
+    <hyperlink ref="F4" r:id="rId5" xr:uid="{9C63F538-5153-4FD4-9FDE-BF86BF0E1EB8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId6"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABC47B48-85A6-4DB0-B46C-2C974E03CC91}">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="9.1796875" style="1"/>
+    <col min="2" max="2" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="144.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.1796875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D2" s="1">
+        <v>225564</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D3" s="1">
+        <v>225564</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D4" s="1">
+        <v>225504</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D13"/>
   <sheetViews>
@@ -1248,7 +1903,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:N3"/>
   <sheetViews>
@@ -1353,7 +2008,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:M3"/>
   <sheetViews>
@@ -1457,7 +2112,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:M3"/>
   <sheetViews>
@@ -1561,7 +2216,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:M3"/>
   <sheetViews>
@@ -1663,108 +2318,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:M3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="12" width="7.7265625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.7265625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>